<commit_message>
Schmale Breite der Plus in Doku und Groessenvergleichsmodel uebernommen.
</commit_message>
<xml_diff>
--- a/Doku/MPCnew-Größenverhältnisse_20210105.xlsx
+++ b/Doku/MPCnew-Größenverhältnisse_20210105.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0_Daten\Projekte-Sync\MarexOS-RD\32_ENG_Electronics\10_Studies+calculations\Konzept\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Firma\MPCnew_GitHub\Gehaeuse\Doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1692A390-9401-4F2F-9459-809AD9151D6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC6FC33-D3C3-40A9-9D6D-08BA9DEB98A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5CFDBDF0-B665-41A2-A114-7ACC5EBF4BFC}"/>
+    <workbookView xWindow="0" yWindow="608" windowWidth="15923" windowHeight="12472" xr2:uid="{5CFDBDF0-B665-41A2-A114-7ACC5EBF4BFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Dimensionen" sheetId="4" r:id="rId1"/>
@@ -86,38 +86,38 @@
     <t>PCB M12 MPC 2</t>
   </si>
   <si>
-    <t>05.01.2021
+    <t>MPC 2 Modular</t>
+  </si>
+  <si>
+    <t>PCB Basis MPC 3</t>
+  </si>
+  <si>
+    <t>PCB M12 MPC 3</t>
+  </si>
+  <si>
+    <t>PCB Klemme Wago MPC 3</t>
+  </si>
+  <si>
+    <t>PCB Display MPC 2</t>
+  </si>
+  <si>
+    <t>Einsparung MPC 3 gegenüber MPC 2</t>
+  </si>
+  <si>
+    <t>Bauraum Modular</t>
+  </si>
+  <si>
+    <t>Bauraum Cabinet -&gt; Plus</t>
+  </si>
+  <si>
+    <t>PCB-Fläche Modular Standard</t>
+  </si>
+  <si>
+    <t>PCB-Fläche Modular Extension</t>
+  </si>
+  <si>
+    <t>07.01.2021
 Henkner</t>
-  </si>
-  <si>
-    <t>MPC 2 Modular</t>
-  </si>
-  <si>
-    <t>PCB Basis MPC 3</t>
-  </si>
-  <si>
-    <t>PCB M12 MPC 3</t>
-  </si>
-  <si>
-    <t>PCB Klemme Wago MPC 3</t>
-  </si>
-  <si>
-    <t>PCB Display MPC 2</t>
-  </si>
-  <si>
-    <t>Einsparung MPC 3 gegenüber MPC 2</t>
-  </si>
-  <si>
-    <t>Bauraum Modular</t>
-  </si>
-  <si>
-    <t>Bauraum Cabinet -&gt; Plus</t>
-  </si>
-  <si>
-    <t>PCB-Fläche Modular Standard</t>
-  </si>
-  <si>
-    <t>PCB-Fläche Modular Extension</t>
   </si>
 </sst>
 </file>
@@ -305,19 +305,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -339,6 +327,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -657,98 +657,98 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="7.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="7.59765625" customWidth="1"/>
+    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="7.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="11">
+      <c r="B5" s="7">
         <v>290</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="7">
         <v>170</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="7">
         <v>45</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11">
+      <c r="E5" s="7"/>
+      <c r="F5" s="7">
         <v>320</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="7">
         <v>170</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="7">
         <v>62.5</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="8">
         <f>F5*G5*H5/1000000</f>
         <v>3.4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -771,174 +771,174 @@
       <c r="H6" s="1">
         <v>55.3</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="4">
         <f t="shared" ref="I6:I9" si="0">F6*G6*H6/1000000</f>
         <v>3.1272150000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="11">
         <v>310</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="11">
         <v>240</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="11">
         <v>95</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11">
         <v>350</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="11">
         <v>257</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="11">
         <v>104</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="12">
         <f t="shared" si="0"/>
         <v>9.3547999999999991</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="9">
         <v>215</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="9">
         <v>170</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="9">
         <v>40</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13">
+      <c r="E8" s="9"/>
+      <c r="F8" s="9">
         <v>243</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="9">
         <v>170</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="9">
         <v>45.8</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="10">
         <f t="shared" si="0"/>
         <v>1.8919979999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="13">
         <v>260</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="13">
         <v>170</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="13">
         <v>97</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17">
-        <v>305</v>
-      </c>
-      <c r="G9" s="17">
+      <c r="E9" s="13"/>
+      <c r="F9" s="13">
+        <v>296</v>
+      </c>
+      <c r="G9" s="13">
         <v>180</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="13">
         <v>115</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="14">
         <f t="shared" si="0"/>
-        <v>6.3135000000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+        <v>6.1272000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="7">
         <v>283</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="7">
         <v>162</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="7">
         <v>2</v>
       </c>
-      <c r="E10" s="12">
-        <f>B10*C10/100</f>
+      <c r="E10" s="8">
+        <f t="shared" ref="E10:E17" si="1">B10*C10/100</f>
         <v>458.46</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="7">
         <v>42</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="7">
         <v>57</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="7">
         <v>1.6</v>
       </c>
-      <c r="E11" s="12">
-        <f>B11*C11/100</f>
+      <c r="E11" s="8">
+        <f t="shared" si="1"/>
         <v>23.94</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="11">
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="7">
         <v>116</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="7">
         <v>37</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12">
-        <f>B12*C12/100</f>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8">
+        <f t="shared" si="1"/>
         <v>42.92</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="13">
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="9">
         <v>154</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="9">
         <v>123</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="9">
         <v>2</v>
       </c>
-      <c r="E13" s="14">
-        <f>B13*C13/100</f>
+      <c r="E13" s="10">
+        <f t="shared" si="1"/>
         <v>189.42</v>
       </c>
       <c r="F13" s="1"/>
@@ -946,21 +946,21 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="13">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="9">
         <v>55</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="9">
         <v>123</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="9">
         <v>2</v>
       </c>
-      <c r="E14" s="14">
-        <f>B14*C14/100</f>
+      <c r="E14" s="10">
+        <f t="shared" si="1"/>
         <v>67.650000000000006</v>
       </c>
       <c r="F14" s="1"/>
@@ -968,7 +968,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -981,8 +981,8 @@
       <c r="D15" s="1">
         <v>1.6</v>
       </c>
-      <c r="E15" s="8">
-        <f>B15*C15/100</f>
+      <c r="E15" s="4">
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="F15" s="1"/>
@@ -990,21 +990,21 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="13">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="9">
         <v>210</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="9">
         <v>40</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="9">
         <v>2</v>
       </c>
-      <c r="E16" s="14">
-        <f>B16*C16/100</f>
+      <c r="E16" s="10">
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="F16" s="1"/>
@@ -1012,7 +1012,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1025,8 +1025,8 @@
       <c r="D17" s="1">
         <v>2</v>
       </c>
-      <c r="E17" s="8">
-        <f>B17*C17/100</f>
+      <c r="E17" s="4">
+        <f t="shared" si="1"/>
         <v>185.6</v>
       </c>
       <c r="F17" s="1"/>
@@ -1034,49 +1034,49 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="24">
+      <c r="B20" s="19"/>
+      <c r="C20" s="20">
         <f>(I5-I8)/I5</f>
         <v>0.44353000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20">
+        <f>(I7-I9)/I7</f>
+        <v>0.34502073801684691</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A22" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="24">
-        <f>(I7-I9)/I7</f>
-        <v>0.32510582802411586</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="24">
+      <c r="B22" s="19"/>
+      <c r="C22" s="20">
         <f>(E10+E11+E12-E13-E14-E16)/(E10+E11+E12)</f>
         <v>0.35073859742633068</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="24">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A23" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20">
         <f>(E10+E11+E12-E13-E14-E15-E16)/(E10+E11+E12)</f>
         <v>0.2669801263991472</v>
       </c>

</xml_diff>